<commit_message>
Add spaCy Dutch & results
</commit_message>
<xml_diff>
--- a/notebooks/experiments/results.xlsx
+++ b/notebooks/experiments/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bernard\Documents\GitHub\thesis\notebooks\experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FD86F9DA-F1C2-4507-A15D-18A0756F0F86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CBFCAB9-7E29-4AD3-83C9-33EBF0C72AD6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="27345" yWindow="8565" windowWidth="17115" windowHeight="15435" xr2:uid="{3251AB55-BDEF-4AC8-9BFB-5C1BBED6BC57}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
   <si>
     <t>Model</t>
   </si>
@@ -62,42 +62,6 @@
     <t>-</t>
   </si>
   <si>
-    <t>TR-News (all/filtered)</t>
-  </si>
-  <si>
-    <t>0.823 / 0.808</t>
-  </si>
-  <si>
-    <t>0.737 / 0.679</t>
-  </si>
-  <si>
-    <t>0.444 / 0.766</t>
-  </si>
-  <si>
-    <t>0.730 / 0.740</t>
-  </si>
-  <si>
-    <t>0.573 / 0.596</t>
-  </si>
-  <si>
-    <t>LGL (all/filtered)</t>
-  </si>
-  <si>
-    <t>GWN (all/filtered)</t>
-  </si>
-  <si>
-    <t>0.371 / 0.613</t>
-  </si>
-  <si>
-    <t>0.705 / 0.718</t>
-  </si>
-  <si>
-    <t>0.521 / 0.543</t>
-  </si>
-  <si>
-    <t>0.346 / 0.580</t>
-  </si>
-  <si>
     <t>English-only</t>
   </si>
   <si>
@@ -119,66 +83,9 @@
     <t>Dutch-only</t>
   </si>
   <si>
-    <t>0.809 / 0.795</t>
-  </si>
-  <si>
-    <t>0.709 / 0.657</t>
-  </si>
-  <si>
-    <t>0.438 / 0.757</t>
-  </si>
-  <si>
-    <t>0.690 / 0.699</t>
-  </si>
-  <si>
-    <t>0.598 / 0.594</t>
-  </si>
-  <si>
-    <t>0.386 / 0.584</t>
-  </si>
-  <si>
-    <t>0.754 / 0.740</t>
-  </si>
-  <si>
-    <t>0.666 / 0.616</t>
-  </si>
-  <si>
-    <t>0.440 / 0.707</t>
-  </si>
-  <si>
-    <t>0.749 / 0.734</t>
-  </si>
-  <si>
-    <t>0.660 / 0.611</t>
-  </si>
-  <si>
-    <t>0.437 / 0.703</t>
-  </si>
-  <si>
-    <t>flair/dutch-ner-large</t>
-  </si>
-  <si>
-    <t>0.787 / 0.769</t>
-  </si>
-  <si>
     <t>flair/ner-english-large</t>
   </si>
   <si>
-    <t>0.467 / 0.759</t>
-  </si>
-  <si>
-    <t>0.836 / 0.820</t>
-  </si>
-  <si>
-    <t>0.708 / 0.647</t>
-  </si>
-  <si>
-    <t>0.762 / 0.703</t>
-  </si>
-  <si>
-    <t>0.485 / 0.793</t>
-  </si>
-  <si>
     <t>en</t>
   </si>
   <si>
@@ -189,6 +96,36 @@
   </si>
   <si>
     <t>40+ lang</t>
+  </si>
+  <si>
+    <t>GWN (filtered)</t>
+  </si>
+  <si>
+    <t>TR-News (all)</t>
+  </si>
+  <si>
+    <t>LGL (all)</t>
+  </si>
+  <si>
+    <r>
+      <t>flair/dutch-ner-large</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <t>* based on XLM-R</t>
+  </si>
+  <si>
+    <t>spaCy/nl_core_news_lg</t>
   </si>
 </sst>
 </file>
@@ -198,10 +135,17 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -235,30 +179,42 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -573,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6794A339-D9F4-4D34-ABF0-508DFB1001DC}">
-  <dimension ref="B3:I21"/>
+  <dimension ref="B3:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -594,13 +550,13 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="F3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="G3" t="s">
         <v>1</v>
@@ -608,59 +564,62 @@
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="1">
+      <c r="D5" s="7">
+        <v>0.73699999999999999</v>
+      </c>
+      <c r="E5" s="7">
+        <v>0.82299999999999995</v>
+      </c>
+      <c r="F5" s="7">
+        <v>0.76600000000000001</v>
+      </c>
+      <c r="G5" s="8">
         <v>0.371</v>
       </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
+      <c r="I5" s="9"/>
+    </row>
+    <row r="6" spans="2:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="1">
+      <c r="D6" s="8">
+        <v>0.52100000000000002</v>
+      </c>
+      <c r="E6" s="8">
+        <v>0.70499999999999996</v>
+      </c>
+      <c r="F6" s="10">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="G6" s="8">
         <v>0.23599999999999999</v>
       </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
+      <c r="I6" s="9"/>
+    </row>
+    <row r="7" spans="2:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" s="6">
+      <c r="D7" s="8">
+        <v>0.57299999999999995</v>
+      </c>
+      <c r="E7" s="10">
+        <v>0.73</v>
+      </c>
+      <c r="F7" s="8">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="G7" s="7">
         <v>0.45400000000000001</v>
       </c>
+      <c r="I7" s="9"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
@@ -696,171 +655,190 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
+    <row r="10" spans="2:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="14"/>
+      <c r="C10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="7">
+        <v>0.76200000000000001</v>
+      </c>
+      <c r="E10" s="7">
+        <v>0.83599999999999997</v>
+      </c>
+      <c r="F10" s="7">
+        <v>0.79300000000000004</v>
+      </c>
+      <c r="G10" s="7">
+        <v>0.68799999999999994</v>
+      </c>
+      <c r="I10" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D11" s="1">
         <v>0.67700000000000005</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E11" s="1">
         <v>0.67700000000000005</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F11" s="1">
         <v>0.71699999999999997</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="2" t="s">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" t="s">
         <v>22</v>
       </c>
-      <c r="D12" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" t="s">
-        <v>16</v>
-      </c>
-      <c r="G12" t="s">
+      <c r="F13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" t="s">
         <v>1</v>
       </c>
-      <c r="I12" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="G13" s="7">
+      <c r="I13" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="11">
+        <v>0.70899999999999996</v>
+      </c>
+      <c r="E14" s="11">
+        <v>0.80900000000000005</v>
+      </c>
+      <c r="F14" s="11">
+        <v>0.75700000000000001</v>
+      </c>
+      <c r="G14" s="12">
         <v>0.63</v>
       </c>
-      <c r="I13" s="8" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="2"/>
-      <c r="C14" t="s">
-        <v>42</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="G14" s="5">
-        <v>0.68799999999999994</v>
-      </c>
-      <c r="I14" s="8" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G15" s="1">
+      <c r="I14" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="8">
+        <v>0.59799999999999998</v>
+      </c>
+      <c r="E15" s="10">
+        <v>0.69</v>
+      </c>
+      <c r="F15" s="10">
+        <v>0.64</v>
+      </c>
+      <c r="G15" s="8">
         <v>0.53500000000000003</v>
       </c>
-      <c r="I15" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
-        <v>25</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G16" s="3">
+      <c r="I15" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="10">
+        <v>0.66</v>
+      </c>
+      <c r="E16" s="8">
+        <v>0.749</v>
+      </c>
+      <c r="F16" s="8">
+        <v>0.70299999999999996</v>
+      </c>
+      <c r="G16" s="10">
+        <v>0.57599999999999996</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C17" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="8">
+        <v>0.66600000000000004</v>
+      </c>
+      <c r="E17" s="8">
+        <v>0.754</v>
+      </c>
+      <c r="F17" s="8">
+        <v>0.70699999999999996</v>
+      </c>
+      <c r="G17" s="10">
         <v>0.6</v>
       </c>
-      <c r="I16" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
-        <v>26</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G17" s="1">
-        <v>0.57599999999999996</v>
-      </c>
-      <c r="I17" s="4" t="s">
-        <v>48</v>
+      <c r="I17" s="9" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C20" t="s">
-        <v>40</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G20" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="5"/>
+      <c r="C20" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" s="7">
+        <v>0.70799999999999996</v>
+      </c>
+      <c r="E20" s="7">
+        <v>0.78700000000000003</v>
+      </c>
+      <c r="F20" s="7">
+        <v>0.75900000000000001</v>
+      </c>
+      <c r="G20" s="7">
         <v>0.68300000000000005</v>
       </c>
+      <c r="I20" s="9"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
+      <c r="C21" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0.374</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="F21" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="G21" s="1">
+        <v>0.39600000000000002</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B27" s="5"/>
+      <c r="C27" s="5" t="s">
+        <v>25</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>